<commit_message>
docs: atualização da documentação
</commit_message>
<xml_diff>
--- a/Product Backlog/Product Backlog VegVin.xlsx
+++ b/Product Backlog/Product Backlog VegVin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\Desktop\Projetos\Autorais\VegVin\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91AA1A11-9D75-4DE9-A526-02456C8A7BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255F903C-2EF1-4224-89C9-3D39BC12F7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Organização" sheetId="8" r:id="rId1"/>
@@ -2011,7 +2011,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{037C858E-BC2B-4548-973A-9152B148283E}" name="Tabela1" displayName="Tabela1" ref="B2:J19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="13" headerRowBorderDxfId="10" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="B2:J19" xr:uid="{037C858E-BC2B-4548-973A-9152B148283E}"/>
+  <autoFilter ref="B2:J19" xr:uid="{037C858E-BC2B-4548-973A-9152B148283E}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Sprint 1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:J19">
     <sortCondition ref="F2:F19"/>
   </sortState>
@@ -2351,7 +2357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953ECF8B-D5AB-4A43-AAA6-BB9E4A5E2E6C}">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2442,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56EC897-511D-459E-B2A6-5083809C3FA0}">
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
@@ -2635,7 +2641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>23</v>
       </c>
@@ -2664,7 +2670,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>25</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2838,7 +2844,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>30</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>32</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>33</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>34</v>
       </c>

</xml_diff>